<commit_message>
updated versions of both these files
</commit_message>
<xml_diff>
--- a/locations.xlsx
+++ b/locations.xlsx
@@ -8,29 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewdinhtruong/Desktop/AI4SocialGood/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2CA772-0F8A-E04B-AAA2-A20D71F1B392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8034E0-23A4-3C41-AE54-BF79FBEE1055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Location 1</t>
-  </si>
-  <si>
-    <t>Location 2</t>
-  </si>
-  <si>
-    <t>Location 3</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -38,6 +42,15 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>Martin Luther King Jr Library</t>
+  </si>
+  <si>
+    <t>San Jose State University</t>
+  </si>
+  <si>
+    <t>8th &amp; San Fernando</t>
   </si>
 </sst>
 </file>
@@ -407,52 +420,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>37.335479999999997</v>
+        <v>37.3352</v>
       </c>
       <c r="C2">
-        <v>-121.893028</v>
+        <v>-121.8811</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>37.338208000000002</v>
+        <v>37.335500000000003</v>
       </c>
       <c r="C3">
-        <v>-121.886329</v>
+        <v>-121.88500000000001</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>37.774900000000002</v>
+        <v>37.333570000000002</v>
       </c>
       <c r="C4">
-        <v>-122.4194</v>
+        <v>-121.87859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>